<commit_message>
fix bug in exercism_4
</commit_message>
<xml_diff>
--- a/testingDocumentation/exercism_4.xlsx
+++ b/testingDocumentation/exercism_4.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wladw\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\wladw\Documents\GitHub\OlenchenkoVladimir\testingDocumentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -529,9 +529,6 @@
     <t>Всплывает тултип с предложением ознакомиться с соглашением.</t>
   </si>
   <si>
-    <t>Задание итоговой аттестации. Часть 4   "Баг-репорты + тестирование WEB"</t>
-  </si>
-  <si>
     <t>Неверное ограничение максимальной длины в поле "Подтверждение пароля"</t>
   </si>
   <si>
@@ -572,6 +569,10 @@
   </si>
   <si>
     <t>В поле "Эл. Почта" допускается ввод кириллицы</t>
+  </si>
+  <si>
+    <t>Задание итоговой аттестации. Часть 4   "Баг-репорты + тестирование WEB"Задание по теме "Баг-репорты + тестирование WEB".
+Необходимо протестировать функционал формы регистрации https://limelab.tech/test/ по требованиям и завести найденные несоответствия в таблицу ниже.</t>
   </si>
 </sst>
 </file>
@@ -873,6 +874,69 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -882,75 +946,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1173,7 +1176,7 @@
   <dimension ref="A1:N134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26:C28"/>
+      <selection activeCell="I4" sqref="I4:I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1191,33 +1194,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="37"/>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
-      <c r="G1" s="37"/>
-      <c r="H1" s="37"/>
-      <c r="I1" s="38"/>
+      <c r="A1" s="43" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="31"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
       <c r="N1" s="1"/>
     </row>
-    <row r="2" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A2" s="39"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="41"/>
+    <row r="2" spans="1:14" ht="81.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="33"/>
+      <c r="I2" s="34"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -1228,10 +1231,10 @@
       <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="31"/>
+      <c r="C3" s="17"/>
       <c r="D3" s="4" t="s">
         <v>2</v>
       </c>
@@ -1257,29 +1260,29 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+      <c r="A4" s="27">
         <v>1</v>
       </c>
-      <c r="B4" s="19" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="20"/>
-      <c r="D4" s="10" t="s">
+      <c r="B4" s="28" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="19"/>
+      <c r="D4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="10" t="s">
+      <c r="E4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G4" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="H4" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="I4" s="7" t="s">
         <v>16</v>
       </c>
       <c r="J4" s="1"/>
@@ -1289,15 +1292,15 @@
       <c r="N4" s="1"/>
     </row>
     <row r="5" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A5" s="17"/>
-      <c r="B5" s="21"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="17"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="26"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="39"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="35"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
       <c r="L5" s="1"/>
@@ -1305,15 +1308,15 @@
       <c r="N5" s="1"/>
     </row>
     <row r="6" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A6" s="17"/>
-      <c r="B6" s="23"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="26"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="22"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="39"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="35"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
       <c r="L6" s="1"/>
@@ -1321,19 +1324,19 @@
       <c r="N6" s="1"/>
     </row>
     <row r="7" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A7" s="17"/>
-      <c r="B7" s="32" t="s">
+      <c r="A7" s="8"/>
+      <c r="B7" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="33" t="s">
+      <c r="C7" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="26"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="8"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
@@ -1341,17 +1344,17 @@
       <c r="N7" s="1"/>
     </row>
     <row r="8" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A8" s="17"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="18"/>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="10" t="s">
+      <c r="A8" s="8"/>
+      <c r="B8" s="9"/>
+      <c r="C8" s="9"/>
+      <c r="D8" s="9"/>
+      <c r="E8" s="9"/>
+      <c r="F8" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="26"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="8"/>
+      <c r="I8" s="35"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1"/>
@@ -1359,21 +1362,21 @@
       <c r="N8" s="1"/>
     </row>
     <row r="9" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A9" s="17"/>
-      <c r="B9" s="28" t="s">
+      <c r="A9" s="8"/>
+      <c r="B9" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="D9" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="31"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="17"/>
-      <c r="I9" s="26"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="41"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="8"/>
+      <c r="I9" s="35"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
@@ -1381,17 +1384,17 @@
       <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
-      <c r="D10" s="35" t="s">
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E10" s="20"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="17"/>
-      <c r="I10" s="26"/>
+      <c r="E10" s="19"/>
+      <c r="F10" s="42"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
+      <c r="I10" s="35"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
@@ -1399,46 +1402,46 @@
       <c r="N10" s="1"/>
     </row>
     <row r="11" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="17"/>
-      <c r="B11" s="17"/>
-      <c r="C11" s="17"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="22"/>
+      <c r="A11" s="8"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="20"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="6"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="17"/>
-      <c r="I11" s="26"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8"/>
+      <c r="I11" s="35"/>
     </row>
     <row r="12" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A12" s="17"/>
-      <c r="B12" s="17"/>
-      <c r="C12" s="17"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="22"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="20"/>
+      <c r="E12" s="21"/>
       <c r="F12" s="6"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="17"/>
-      <c r="I12" s="26"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8"/>
+      <c r="I12" s="35"/>
     </row>
     <row r="13" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A13" s="18"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="18"/>
-      <c r="D13" s="23"/>
-      <c r="E13" s="24"/>
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+      <c r="D13" s="22"/>
+      <c r="E13" s="23"/>
       <c r="F13" s="6"/>
-      <c r="G13" s="18"/>
-      <c r="H13" s="18"/>
-      <c r="I13" s="27"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="36"/>
     </row>
     <row r="14" spans="1:14" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C14" s="31"/>
+      <c r="C14" s="17"/>
       <c r="D14" s="4" t="s">
         <v>2</v>
       </c>
@@ -1459,151 +1462,151 @@
       </c>
     </row>
     <row r="15" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A15" s="16">
+      <c r="A15" s="27">
         <v>2</v>
       </c>
-      <c r="B15" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="10" t="s">
+      <c r="B15" s="28" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="E15" s="10" t="s">
+      <c r="E15" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="G15" s="10" t="s">
+      <c r="G15" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="H15" s="10" t="s">
+      <c r="H15" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="I15" s="10" t="s">
+      <c r="I15" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="15" x14ac:dyDescent="0.2">
-      <c r="A16" s="17"/>
-      <c r="B16" s="21"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="14"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="26"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="20"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8"/>
+      <c r="I16" s="35"/>
     </row>
     <row r="17" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A17" s="17"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="17"/>
+      <c r="A17" s="8"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
       <c r="F17" s="5"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="17"/>
-      <c r="I17" s="26"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="35"/>
     </row>
     <row r="18" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A18" s="17"/>
-      <c r="B18" s="32" t="s">
+      <c r="A18" s="8"/>
+      <c r="B18" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="33" t="s">
+      <c r="C18" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="17"/>
-      <c r="E18" s="17"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
       <c r="F18" s="5"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="17"/>
-      <c r="I18" s="26"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="35"/>
     </row>
     <row r="19" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A19" s="17"/>
-      <c r="B19" s="18"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="18"/>
-      <c r="E19" s="18"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
       <c r="F19" s="5"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="17"/>
-      <c r="I19" s="26"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="8"/>
+      <c r="I19" s="35"/>
     </row>
     <row r="20" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A20" s="17"/>
-      <c r="B20" s="28" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="D20" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E20" s="31"/>
+      <c r="E20" s="17"/>
       <c r="F20" s="5"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="17"/>
-      <c r="I20" s="26"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="35"/>
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A21" s="17"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="17"/>
-      <c r="D21" s="35" t="s">
+      <c r="A21" s="8"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="20"/>
+      <c r="E21" s="19"/>
       <c r="F21" s="5"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="17"/>
-      <c r="I21" s="26"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="8"/>
+      <c r="I21" s="35"/>
     </row>
     <row r="22" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A22" s="17"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="17"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="22"/>
+      <c r="A22" s="8"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="21"/>
       <c r="F22" s="5"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="17"/>
-      <c r="I22" s="26"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="8"/>
+      <c r="I22" s="35"/>
     </row>
     <row r="23" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="17"/>
-      <c r="D23" s="21"/>
-      <c r="E23" s="22"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="20"/>
+      <c r="E23" s="21"/>
       <c r="F23" s="5"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="17"/>
-      <c r="I23" s="26"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="8"/>
+      <c r="I23" s="35"/>
     </row>
     <row r="24" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A24" s="18"/>
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="24"/>
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="23"/>
       <c r="F24" s="5"/>
-      <c r="G24" s="18"/>
-      <c r="H24" s="18"/>
-      <c r="I24" s="27"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="36"/>
     </row>
     <row r="25" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="31"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="4" t="s">
         <v>2</v>
       </c>
@@ -1624,153 +1627,153 @@
       </c>
     </row>
     <row r="26" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A26" s="16">
+      <c r="A26" s="27">
         <v>3</v>
       </c>
-      <c r="B26" s="19" t="s">
-        <v>77</v>
-      </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="10" t="s">
+      <c r="B26" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26" s="19"/>
+      <c r="D26" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="10" t="s">
+      <c r="E26" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F26" s="13" t="s">
+      <c r="F26" s="14" t="s">
         <v>27</v>
       </c>
-      <c r="G26" s="10" t="s">
+      <c r="G26" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H26" s="10" t="s">
+      <c r="H26" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I26" s="10" t="s">
+      <c r="I26" s="7" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A27" s="17"/>
-      <c r="B27" s="21"/>
-      <c r="C27" s="22"/>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="17"/>
-      <c r="I27" s="26"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="37"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="8"/>
+      <c r="I27" s="35"/>
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A28" s="17"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
-      <c r="F28" s="14"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="17"/>
-      <c r="I28" s="26"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+      <c r="F28" s="15"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="8"/>
+      <c r="I28" s="35"/>
     </row>
     <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A29" s="17"/>
-      <c r="B29" s="32" t="s">
+      <c r="A29" s="8"/>
+      <c r="B29" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C29" s="33" t="s">
+      <c r="C29" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-      <c r="F29" s="10" t="s">
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="G29" s="17"/>
-      <c r="H29" s="17"/>
-      <c r="I29" s="26"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="35"/>
     </row>
     <row r="30" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A30" s="17"/>
-      <c r="B30" s="18"/>
-      <c r="C30" s="18"/>
-      <c r="D30" s="18"/>
-      <c r="E30" s="18"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="17"/>
-      <c r="I30" s="26"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="F30" s="41"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="8"/>
+      <c r="I30" s="35"/>
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A31" s="17"/>
-      <c r="B31" s="28" t="s">
+      <c r="A31" s="8"/>
+      <c r="B31" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="29" t="s">
+      <c r="C31" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D31" s="34" t="s">
+      <c r="D31" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E31" s="31"/>
-      <c r="F31" s="12"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="17"/>
-      <c r="I31" s="26"/>
+      <c r="E31" s="17"/>
+      <c r="F31" s="42"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="35"/>
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A32" s="17"/>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="35" t="s">
+      <c r="A32" s="8"/>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E32" s="20"/>
+      <c r="E32" s="19"/>
       <c r="F32" s="5"/>
-      <c r="G32" s="17"/>
-      <c r="H32" s="17"/>
-      <c r="I32" s="26"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="8"/>
+      <c r="I32" s="35"/>
     </row>
     <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A33" s="17"/>
-      <c r="B33" s="17"/>
-      <c r="C33" s="17"/>
-      <c r="D33" s="21"/>
-      <c r="E33" s="22"/>
+      <c r="A33" s="8"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="21"/>
       <c r="F33" s="5"/>
-      <c r="G33" s="17"/>
-      <c r="H33" s="17"/>
-      <c r="I33" s="26"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="35"/>
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A34" s="17"/>
-      <c r="B34" s="17"/>
-      <c r="C34" s="17"/>
-      <c r="D34" s="21"/>
-      <c r="E34" s="22"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="21"/>
       <c r="F34" s="5"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="26"/>
+      <c r="G34" s="8"/>
+      <c r="H34" s="8"/>
+      <c r="I34" s="35"/>
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A35" s="18"/>
-      <c r="B35" s="18"/>
-      <c r="C35" s="18"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="24"/>
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="22"/>
+      <c r="E35" s="23"/>
       <c r="F35" s="5"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="27"/>
+      <c r="G35" s="9"/>
+      <c r="H35" s="9"/>
+      <c r="I35" s="36"/>
     </row>
     <row r="36" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C36" s="31"/>
+      <c r="C36" s="17"/>
       <c r="D36" s="4" t="s">
         <v>2</v>
       </c>
@@ -1791,151 +1794,151 @@
       </c>
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="16">
+      <c r="A37" s="27">
         <v>4</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>66</v>
-      </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="10" t="s">
+      <c r="B37" s="28" t="s">
+        <v>65</v>
+      </c>
+      <c r="C37" s="19"/>
+      <c r="D37" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="E37" s="10" t="s">
+      <c r="E37" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F37" s="13" t="s">
+      <c r="F37" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="G37" s="10" t="s">
+      <c r="G37" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H37" s="10" t="s">
+      <c r="H37" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="I37" s="10" t="s">
+      <c r="I37" s="7" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="38" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="17"/>
-      <c r="B38" s="21"/>
-      <c r="C38" s="22"/>
-      <c r="D38" s="17"/>
-      <c r="E38" s="17"/>
-      <c r="F38" s="15"/>
-      <c r="G38" s="17"/>
-      <c r="H38" s="17"/>
-      <c r="I38" s="26"/>
+      <c r="A38" s="8"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="8"/>
+      <c r="E38" s="8"/>
+      <c r="F38" s="37"/>
+      <c r="G38" s="8"/>
+      <c r="H38" s="8"/>
+      <c r="I38" s="35"/>
     </row>
     <row r="39" spans="1:9" ht="47.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="17"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="17"/>
-      <c r="E39" s="17"/>
-      <c r="F39" s="15"/>
-      <c r="G39" s="17"/>
-      <c r="H39" s="17"/>
-      <c r="I39" s="26"/>
+      <c r="A39" s="8"/>
+      <c r="B39" s="22"/>
+      <c r="C39" s="23"/>
+      <c r="D39" s="8"/>
+      <c r="E39" s="8"/>
+      <c r="F39" s="37"/>
+      <c r="G39" s="8"/>
+      <c r="H39" s="8"/>
+      <c r="I39" s="35"/>
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A40" s="17"/>
-      <c r="B40" s="32" t="s">
+      <c r="A40" s="8"/>
+      <c r="B40" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C40" s="33" t="s">
+      <c r="C40" s="29" t="s">
         <v>35</v>
       </c>
-      <c r="D40" s="17"/>
-      <c r="E40" s="17"/>
-      <c r="F40" s="14"/>
-      <c r="G40" s="17"/>
-      <c r="H40" s="17"/>
-      <c r="I40" s="26"/>
+      <c r="D40" s="8"/>
+      <c r="E40" s="8"/>
+      <c r="F40" s="15"/>
+      <c r="G40" s="8"/>
+      <c r="H40" s="8"/>
+      <c r="I40" s="35"/>
     </row>
     <row r="41" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="17"/>
-      <c r="B41" s="18"/>
-      <c r="C41" s="18"/>
-      <c r="D41" s="18"/>
-      <c r="E41" s="18"/>
+      <c r="A41" s="8"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="9"/>
       <c r="F41" s="5"/>
-      <c r="G41" s="17"/>
-      <c r="H41" s="17"/>
-      <c r="I41" s="26"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="35"/>
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A42" s="17"/>
-      <c r="B42" s="28" t="s">
+      <c r="A42" s="8"/>
+      <c r="B42" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C42" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D42" s="34" t="s">
+      <c r="D42" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E42" s="31"/>
+      <c r="E42" s="17"/>
       <c r="F42" s="5"/>
-      <c r="G42" s="17"/>
-      <c r="H42" s="17"/>
-      <c r="I42" s="26"/>
+      <c r="G42" s="8"/>
+      <c r="H42" s="8"/>
+      <c r="I42" s="35"/>
     </row>
     <row r="43" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="17"/>
-      <c r="B43" s="17"/>
-      <c r="C43" s="17"/>
-      <c r="D43" s="35" t="s">
+      <c r="A43" s="8"/>
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E43" s="20"/>
+      <c r="E43" s="19"/>
       <c r="F43" s="5"/>
-      <c r="G43" s="17"/>
-      <c r="H43" s="17"/>
-      <c r="I43" s="26"/>
+      <c r="G43" s="8"/>
+      <c r="H43" s="8"/>
+      <c r="I43" s="35"/>
     </row>
     <row r="44" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="17"/>
-      <c r="B44" s="17"/>
-      <c r="C44" s="17"/>
-      <c r="D44" s="21"/>
-      <c r="E44" s="22"/>
+      <c r="A44" s="8"/>
+      <c r="B44" s="8"/>
+      <c r="C44" s="8"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="21"/>
       <c r="F44" s="5"/>
-      <c r="G44" s="17"/>
-      <c r="H44" s="17"/>
-      <c r="I44" s="26"/>
+      <c r="G44" s="8"/>
+      <c r="H44" s="8"/>
+      <c r="I44" s="35"/>
     </row>
     <row r="45" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="17"/>
-      <c r="B45" s="17"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="21"/>
-      <c r="E45" s="22"/>
+      <c r="A45" s="8"/>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="21"/>
       <c r="F45" s="5"/>
-      <c r="G45" s="17"/>
-      <c r="H45" s="17"/>
-      <c r="I45" s="26"/>
+      <c r="G45" s="8"/>
+      <c r="H45" s="8"/>
+      <c r="I45" s="35"/>
     </row>
     <row r="46" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="18"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="18"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="24"/>
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="22"/>
+      <c r="E46" s="23"/>
       <c r="F46" s="5"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="27"/>
+      <c r="G46" s="9"/>
+      <c r="H46" s="9"/>
+      <c r="I46" s="36"/>
     </row>
     <row r="47" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A47" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C47" s="31"/>
+      <c r="C47" s="17"/>
       <c r="D47" s="4" t="s">
         <v>2</v>
       </c>
@@ -1956,151 +1959,151 @@
       </c>
     </row>
     <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="16">
+      <c r="A48" s="27">
         <v>5</v>
       </c>
-      <c r="B48" s="19" t="s">
+      <c r="B48" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="19"/>
+      <c r="D48" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="C48" s="20"/>
-      <c r="D48" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="E48" s="10" t="s">
+      <c r="E48" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F48" s="13" t="s">
+      <c r="F48" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G48" s="10" t="s">
+      <c r="G48" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H48" s="10" t="s">
+      <c r="H48" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I48" s="10" t="s">
+      <c r="I48" s="7" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="17"/>
-      <c r="B49" s="21"/>
-      <c r="C49" s="22"/>
-      <c r="D49" s="17"/>
-      <c r="E49" s="17"/>
-      <c r="F49" s="15"/>
-      <c r="G49" s="17"/>
-      <c r="H49" s="17"/>
-      <c r="I49" s="26"/>
+      <c r="A49" s="8"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="8"/>
+      <c r="E49" s="8"/>
+      <c r="F49" s="37"/>
+      <c r="G49" s="8"/>
+      <c r="H49" s="8"/>
+      <c r="I49" s="35"/>
     </row>
     <row r="50" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="17"/>
-      <c r="B50" s="23"/>
-      <c r="C50" s="24"/>
-      <c r="D50" s="17"/>
-      <c r="E50" s="17"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="17"/>
-      <c r="H50" s="17"/>
-      <c r="I50" s="26"/>
+      <c r="A50" s="8"/>
+      <c r="B50" s="22"/>
+      <c r="C50" s="23"/>
+      <c r="D50" s="8"/>
+      <c r="E50" s="8"/>
+      <c r="F50" s="15"/>
+      <c r="G50" s="8"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="35"/>
     </row>
     <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="17"/>
-      <c r="B51" s="32" t="s">
+      <c r="A51" s="8"/>
+      <c r="B51" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C51" s="33" t="s">
+      <c r="C51" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="D51" s="17"/>
-      <c r="E51" s="17"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8"/>
       <c r="F51" s="5"/>
-      <c r="G51" s="17"/>
-      <c r="H51" s="17"/>
-      <c r="I51" s="26"/>
+      <c r="G51" s="8"/>
+      <c r="H51" s="8"/>
+      <c r="I51" s="35"/>
     </row>
     <row r="52" spans="1:9" ht="54" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="17"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="18"/>
-      <c r="D52" s="18"/>
-      <c r="E52" s="18"/>
+      <c r="A52" s="8"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="9"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
       <c r="F52" s="5"/>
-      <c r="G52" s="17"/>
-      <c r="H52" s="17"/>
-      <c r="I52" s="26"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="35"/>
     </row>
     <row r="53" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="17"/>
-      <c r="B53" s="28" t="s">
+      <c r="A53" s="8"/>
+      <c r="B53" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C53" s="29" t="s">
+      <c r="C53" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D53" s="34" t="s">
+      <c r="D53" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E53" s="31"/>
+      <c r="E53" s="17"/>
       <c r="F53" s="5"/>
-      <c r="G53" s="17"/>
-      <c r="H53" s="17"/>
-      <c r="I53" s="26"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="35"/>
     </row>
     <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A54" s="17"/>
-      <c r="B54" s="17"/>
-      <c r="C54" s="17"/>
-      <c r="D54" s="35" t="s">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E54" s="20"/>
+      <c r="E54" s="19"/>
       <c r="F54" s="5"/>
-      <c r="G54" s="17"/>
-      <c r="H54" s="17"/>
-      <c r="I54" s="26"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="35"/>
     </row>
     <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A55" s="17"/>
-      <c r="B55" s="17"/>
-      <c r="C55" s="17"/>
-      <c r="D55" s="21"/>
-      <c r="E55" s="22"/>
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="20"/>
+      <c r="E55" s="21"/>
       <c r="F55" s="5"/>
-      <c r="G55" s="17"/>
-      <c r="H55" s="17"/>
-      <c r="I55" s="26"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="35"/>
     </row>
     <row r="56" spans="1:9" ht="0.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="17"/>
-      <c r="B56" s="17"/>
-      <c r="C56" s="17"/>
-      <c r="D56" s="21"/>
-      <c r="E56" s="22"/>
+      <c r="A56" s="8"/>
+      <c r="B56" s="8"/>
+      <c r="C56" s="8"/>
+      <c r="D56" s="20"/>
+      <c r="E56" s="21"/>
       <c r="F56" s="5"/>
-      <c r="G56" s="17"/>
-      <c r="H56" s="17"/>
-      <c r="I56" s="26"/>
+      <c r="G56" s="8"/>
+      <c r="H56" s="8"/>
+      <c r="I56" s="35"/>
     </row>
     <row r="57" spans="1:9" ht="15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="18"/>
-      <c r="B57" s="18"/>
-      <c r="C57" s="18"/>
-      <c r="D57" s="23"/>
-      <c r="E57" s="24"/>
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="22"/>
+      <c r="E57" s="23"/>
       <c r="F57" s="5"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="18"/>
-      <c r="I57" s="27"/>
+      <c r="G57" s="9"/>
+      <c r="H57" s="9"/>
+      <c r="I57" s="36"/>
     </row>
     <row r="58" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A58" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B58" s="30" t="s">
+      <c r="B58" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C58" s="31"/>
+      <c r="C58" s="17"/>
       <c r="D58" s="4" t="s">
         <v>2</v>
       </c>
@@ -2121,151 +2124,151 @@
       </c>
     </row>
     <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A59" s="16">
+      <c r="A59" s="27">
         <v>6</v>
       </c>
-      <c r="B59" s="19" t="s">
+      <c r="B59" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C59" s="19"/>
+      <c r="D59" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="C59" s="20"/>
-      <c r="D59" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="E59" s="10" t="s">
+      <c r="E59" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="F59" s="13" t="s">
+      <c r="F59" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G59" s="10" t="s">
+      <c r="G59" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="H59" s="10" t="s">
+      <c r="H59" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="I59" s="10" t="s">
+      <c r="I59" s="7" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="17"/>
-      <c r="B60" s="21"/>
-      <c r="C60" s="22"/>
-      <c r="D60" s="17"/>
-      <c r="E60" s="17"/>
-      <c r="F60" s="14"/>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="26"/>
+      <c r="A60" s="8"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="8"/>
+      <c r="E60" s="8"/>
+      <c r="F60" s="15"/>
+      <c r="G60" s="8"/>
+      <c r="H60" s="8"/>
+      <c r="I60" s="35"/>
     </row>
     <row r="61" spans="1:9" ht="63.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="17"/>
-      <c r="B61" s="23"/>
-      <c r="C61" s="24"/>
-      <c r="D61" s="17"/>
-      <c r="E61" s="17"/>
+      <c r="A61" s="8"/>
+      <c r="B61" s="22"/>
+      <c r="C61" s="23"/>
+      <c r="D61" s="8"/>
+      <c r="E61" s="8"/>
       <c r="F61" s="5"/>
-      <c r="G61" s="17"/>
-      <c r="H61" s="17"/>
-      <c r="I61" s="26"/>
+      <c r="G61" s="8"/>
+      <c r="H61" s="8"/>
+      <c r="I61" s="35"/>
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A62" s="17"/>
-      <c r="B62" s="32" t="s">
+      <c r="A62" s="8"/>
+      <c r="B62" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C62" s="33" t="s">
+      <c r="C62" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D62" s="17"/>
-      <c r="E62" s="17"/>
+      <c r="D62" s="8"/>
+      <c r="E62" s="8"/>
       <c r="F62" s="5"/>
-      <c r="G62" s="17"/>
-      <c r="H62" s="17"/>
-      <c r="I62" s="26"/>
+      <c r="G62" s="8"/>
+      <c r="H62" s="8"/>
+      <c r="I62" s="35"/>
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A63" s="17"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="18"/>
-      <c r="D63" s="18"/>
-      <c r="E63" s="18"/>
+      <c r="A63" s="8"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="9"/>
+      <c r="D63" s="9"/>
+      <c r="E63" s="9"/>
       <c r="F63" s="5"/>
-      <c r="G63" s="17"/>
-      <c r="H63" s="17"/>
-      <c r="I63" s="26"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="35"/>
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A64" s="17"/>
-      <c r="B64" s="28" t="s">
+      <c r="A64" s="8"/>
+      <c r="B64" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C64" s="29" t="s">
+      <c r="C64" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D64" s="34" t="s">
+      <c r="D64" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E64" s="31"/>
+      <c r="E64" s="17"/>
       <c r="F64" s="5"/>
-      <c r="G64" s="17"/>
-      <c r="H64" s="17"/>
-      <c r="I64" s="26"/>
+      <c r="G64" s="8"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="35"/>
     </row>
     <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="17"/>
-      <c r="B65" s="17"/>
-      <c r="C65" s="17"/>
-      <c r="D65" s="35" t="s">
+      <c r="A65" s="8"/>
+      <c r="B65" s="8"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E65" s="20"/>
+      <c r="E65" s="19"/>
       <c r="F65" s="5"/>
-      <c r="G65" s="17"/>
-      <c r="H65" s="17"/>
-      <c r="I65" s="26"/>
+      <c r="G65" s="8"/>
+      <c r="H65" s="8"/>
+      <c r="I65" s="35"/>
     </row>
     <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="17"/>
-      <c r="B66" s="17"/>
-      <c r="C66" s="17"/>
-      <c r="D66" s="21"/>
-      <c r="E66" s="22"/>
+      <c r="A66" s="8"/>
+      <c r="B66" s="8"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="20"/>
+      <c r="E66" s="21"/>
       <c r="F66" s="5"/>
-      <c r="G66" s="17"/>
-      <c r="H66" s="17"/>
-      <c r="I66" s="26"/>
+      <c r="G66" s="8"/>
+      <c r="H66" s="8"/>
+      <c r="I66" s="35"/>
     </row>
     <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A67" s="17"/>
-      <c r="B67" s="17"/>
-      <c r="C67" s="17"/>
-      <c r="D67" s="21"/>
-      <c r="E67" s="22"/>
+      <c r="A67" s="8"/>
+      <c r="B67" s="8"/>
+      <c r="C67" s="8"/>
+      <c r="D67" s="20"/>
+      <c r="E67" s="21"/>
       <c r="F67" s="5"/>
-      <c r="G67" s="17"/>
-      <c r="H67" s="17"/>
-      <c r="I67" s="26"/>
+      <c r="G67" s="8"/>
+      <c r="H67" s="8"/>
+      <c r="I67" s="35"/>
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A68" s="18"/>
-      <c r="B68" s="18"/>
-      <c r="C68" s="18"/>
-      <c r="D68" s="23"/>
-      <c r="E68" s="24"/>
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="22"/>
+      <c r="E68" s="23"/>
       <c r="F68" s="5"/>
-      <c r="G68" s="18"/>
-      <c r="H68" s="18"/>
-      <c r="I68" s="27"/>
+      <c r="G68" s="9"/>
+      <c r="H68" s="9"/>
+      <c r="I68" s="36"/>
     </row>
     <row r="69" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A69" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B69" s="30" t="s">
+      <c r="B69" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C69" s="31"/>
+      <c r="C69" s="17"/>
       <c r="D69" s="4" t="s">
         <v>2</v>
       </c>
@@ -2286,151 +2289,151 @@
       </c>
     </row>
     <row r="70" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="16">
+      <c r="A70" s="27">
         <v>7</v>
       </c>
-      <c r="B70" s="19" t="s">
-        <v>71</v>
-      </c>
-      <c r="C70" s="20"/>
-      <c r="D70" s="10" t="s">
+      <c r="B70" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" s="19"/>
+      <c r="D70" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="E70" s="10" t="s">
+      <c r="E70" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F70" s="13" t="s">
+      <c r="F70" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="G70" s="10" t="s">
+      <c r="G70" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="H70" s="10" t="s">
+      <c r="H70" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="I70" s="10" t="s">
+      <c r="I70" s="7" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="71" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="17"/>
-      <c r="B71" s="21"/>
-      <c r="C71" s="22"/>
-      <c r="D71" s="17"/>
-      <c r="E71" s="17"/>
-      <c r="F71" s="14"/>
-      <c r="G71" s="17"/>
-      <c r="H71" s="17"/>
-      <c r="I71" s="26"/>
+      <c r="A71" s="8"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="8"/>
+      <c r="E71" s="8"/>
+      <c r="F71" s="15"/>
+      <c r="G71" s="8"/>
+      <c r="H71" s="8"/>
+      <c r="I71" s="35"/>
     </row>
     <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="17"/>
-      <c r="B72" s="23"/>
-      <c r="C72" s="24"/>
-      <c r="D72" s="17"/>
-      <c r="E72" s="17"/>
+      <c r="A72" s="8"/>
+      <c r="B72" s="22"/>
+      <c r="C72" s="23"/>
+      <c r="D72" s="8"/>
+      <c r="E72" s="8"/>
       <c r="F72" s="5"/>
-      <c r="G72" s="17"/>
-      <c r="H72" s="17"/>
-      <c r="I72" s="26"/>
+      <c r="G72" s="8"/>
+      <c r="H72" s="8"/>
+      <c r="I72" s="35"/>
     </row>
     <row r="73" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="17"/>
-      <c r="B73" s="32" t="s">
+      <c r="A73" s="8"/>
+      <c r="B73" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C73" s="33" t="s">
+      <c r="C73" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D73" s="17"/>
-      <c r="E73" s="17"/>
+      <c r="D73" s="8"/>
+      <c r="E73" s="8"/>
       <c r="F73" s="5"/>
-      <c r="G73" s="17"/>
-      <c r="H73" s="17"/>
-      <c r="I73" s="26"/>
+      <c r="G73" s="8"/>
+      <c r="H73" s="8"/>
+      <c r="I73" s="35"/>
     </row>
     <row r="74" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="17"/>
-      <c r="B74" s="18"/>
-      <c r="C74" s="18"/>
-      <c r="D74" s="18"/>
-      <c r="E74" s="18"/>
+      <c r="A74" s="8"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="9"/>
+      <c r="D74" s="9"/>
+      <c r="E74" s="9"/>
       <c r="F74" s="5"/>
-      <c r="G74" s="17"/>
-      <c r="H74" s="17"/>
-      <c r="I74" s="26"/>
+      <c r="G74" s="8"/>
+      <c r="H74" s="8"/>
+      <c r="I74" s="35"/>
     </row>
     <row r="75" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A75" s="17"/>
-      <c r="B75" s="28" t="s">
+      <c r="A75" s="8"/>
+      <c r="B75" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C75" s="29" t="s">
+      <c r="C75" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D75" s="34" t="s">
+      <c r="D75" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E75" s="31"/>
+      <c r="E75" s="17"/>
       <c r="F75" s="5"/>
-      <c r="G75" s="17"/>
-      <c r="H75" s="17"/>
-      <c r="I75" s="26"/>
+      <c r="G75" s="8"/>
+      <c r="H75" s="8"/>
+      <c r="I75" s="35"/>
     </row>
     <row r="76" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A76" s="17"/>
-      <c r="B76" s="17"/>
-      <c r="C76" s="17"/>
-      <c r="D76" s="35" t="s">
+      <c r="A76" s="8"/>
+      <c r="B76" s="8"/>
+      <c r="C76" s="8"/>
+      <c r="D76" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E76" s="20"/>
+      <c r="E76" s="19"/>
       <c r="F76" s="5"/>
-      <c r="G76" s="17"/>
-      <c r="H76" s="17"/>
-      <c r="I76" s="26"/>
+      <c r="G76" s="8"/>
+      <c r="H76" s="8"/>
+      <c r="I76" s="35"/>
     </row>
     <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A77" s="17"/>
-      <c r="B77" s="17"/>
-      <c r="C77" s="17"/>
-      <c r="D77" s="21"/>
-      <c r="E77" s="22"/>
+      <c r="A77" s="8"/>
+      <c r="B77" s="8"/>
+      <c r="C77" s="8"/>
+      <c r="D77" s="20"/>
+      <c r="E77" s="21"/>
       <c r="F77" s="5"/>
-      <c r="G77" s="17"/>
-      <c r="H77" s="17"/>
-      <c r="I77" s="26"/>
+      <c r="G77" s="8"/>
+      <c r="H77" s="8"/>
+      <c r="I77" s="35"/>
     </row>
     <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A78" s="17"/>
-      <c r="B78" s="17"/>
-      <c r="C78" s="17"/>
-      <c r="D78" s="21"/>
-      <c r="E78" s="22"/>
+      <c r="A78" s="8"/>
+      <c r="B78" s="8"/>
+      <c r="C78" s="8"/>
+      <c r="D78" s="20"/>
+      <c r="E78" s="21"/>
       <c r="F78" s="5"/>
-      <c r="G78" s="17"/>
-      <c r="H78" s="17"/>
-      <c r="I78" s="26"/>
+      <c r="G78" s="8"/>
+      <c r="H78" s="8"/>
+      <c r="I78" s="35"/>
     </row>
     <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A79" s="18"/>
-      <c r="B79" s="18"/>
-      <c r="C79" s="18"/>
-      <c r="D79" s="23"/>
-      <c r="E79" s="24"/>
+      <c r="A79" s="9"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="9"/>
+      <c r="D79" s="22"/>
+      <c r="E79" s="23"/>
       <c r="F79" s="5"/>
-      <c r="G79" s="18"/>
-      <c r="H79" s="18"/>
-      <c r="I79" s="27"/>
+      <c r="G79" s="9"/>
+      <c r="H79" s="9"/>
+      <c r="I79" s="36"/>
     </row>
     <row r="80" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A80" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B80" s="30" t="s">
+      <c r="B80" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C80" s="31"/>
+      <c r="C80" s="17"/>
       <c r="D80" s="4" t="s">
         <v>2</v>
       </c>
@@ -2451,151 +2454,151 @@
       </c>
     </row>
     <row r="81" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="16">
+      <c r="A81" s="27">
         <v>8</v>
       </c>
-      <c r="B81" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="C81" s="20"/>
-      <c r="D81" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="E81" s="10" t="s">
+      <c r="B81" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C81" s="19"/>
+      <c r="D81" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E81" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F81" s="13" t="s">
+      <c r="F81" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="G81" s="10" t="s">
+      <c r="G81" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="H81" s="10" t="s">
+      <c r="H81" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="I81" s="10" t="s">
+      <c r="I81" s="7" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A82" s="17"/>
-      <c r="B82" s="21"/>
-      <c r="C82" s="22"/>
-      <c r="D82" s="17"/>
-      <c r="E82" s="17"/>
-      <c r="F82" s="15"/>
-      <c r="G82" s="17"/>
-      <c r="H82" s="17"/>
-      <c r="I82" s="26"/>
+      <c r="A82" s="8"/>
+      <c r="B82" s="20"/>
+      <c r="C82" s="21"/>
+      <c r="D82" s="8"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="37"/>
+      <c r="G82" s="8"/>
+      <c r="H82" s="8"/>
+      <c r="I82" s="35"/>
     </row>
     <row r="83" spans="1:9" ht="23.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="17"/>
-      <c r="B83" s="23"/>
-      <c r="C83" s="24"/>
-      <c r="D83" s="17"/>
-      <c r="E83" s="17"/>
-      <c r="F83" s="15"/>
-      <c r="G83" s="17"/>
-      <c r="H83" s="17"/>
-      <c r="I83" s="26"/>
+      <c r="A83" s="8"/>
+      <c r="B83" s="22"/>
+      <c r="C83" s="23"/>
+      <c r="D83" s="8"/>
+      <c r="E83" s="8"/>
+      <c r="F83" s="37"/>
+      <c r="G83" s="8"/>
+      <c r="H83" s="8"/>
+      <c r="I83" s="35"/>
     </row>
     <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A84" s="17"/>
-      <c r="B84" s="32" t="s">
+      <c r="A84" s="8"/>
+      <c r="B84" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C84" s="33" t="s">
+      <c r="C84" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D84" s="17"/>
-      <c r="E84" s="17"/>
-      <c r="F84" s="14"/>
-      <c r="G84" s="17"/>
-      <c r="H84" s="17"/>
-      <c r="I84" s="26"/>
+      <c r="D84" s="8"/>
+      <c r="E84" s="8"/>
+      <c r="F84" s="15"/>
+      <c r="G84" s="8"/>
+      <c r="H84" s="8"/>
+      <c r="I84" s="35"/>
     </row>
     <row r="85" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="17"/>
-      <c r="B85" s="18"/>
-      <c r="C85" s="18"/>
-      <c r="D85" s="18"/>
-      <c r="E85" s="18"/>
+      <c r="A85" s="8"/>
+      <c r="B85" s="9"/>
+      <c r="C85" s="9"/>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9"/>
       <c r="F85" s="5"/>
-      <c r="G85" s="17"/>
-      <c r="H85" s="17"/>
-      <c r="I85" s="26"/>
+      <c r="G85" s="8"/>
+      <c r="H85" s="8"/>
+      <c r="I85" s="35"/>
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A86" s="17"/>
-      <c r="B86" s="28" t="s">
+      <c r="A86" s="8"/>
+      <c r="B86" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C86" s="29" t="s">
+      <c r="C86" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D86" s="34" t="s">
+      <c r="D86" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E86" s="31"/>
+      <c r="E86" s="17"/>
       <c r="F86" s="5"/>
-      <c r="G86" s="17"/>
-      <c r="H86" s="17"/>
-      <c r="I86" s="26"/>
+      <c r="G86" s="8"/>
+      <c r="H86" s="8"/>
+      <c r="I86" s="35"/>
     </row>
     <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A87" s="17"/>
-      <c r="B87" s="17"/>
-      <c r="C87" s="17"/>
-      <c r="D87" s="35" t="s">
+      <c r="A87" s="8"/>
+      <c r="B87" s="8"/>
+      <c r="C87" s="8"/>
+      <c r="D87" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E87" s="20"/>
+      <c r="E87" s="19"/>
       <c r="F87" s="5"/>
-      <c r="G87" s="17"/>
-      <c r="H87" s="17"/>
-      <c r="I87" s="26"/>
+      <c r="G87" s="8"/>
+      <c r="H87" s="8"/>
+      <c r="I87" s="35"/>
     </row>
     <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A88" s="17"/>
-      <c r="B88" s="17"/>
-      <c r="C88" s="17"/>
-      <c r="D88" s="21"/>
-      <c r="E88" s="22"/>
+      <c r="A88" s="8"/>
+      <c r="B88" s="8"/>
+      <c r="C88" s="8"/>
+      <c r="D88" s="20"/>
+      <c r="E88" s="21"/>
       <c r="F88" s="5"/>
-      <c r="G88" s="17"/>
-      <c r="H88" s="17"/>
-      <c r="I88" s="26"/>
+      <c r="G88" s="8"/>
+      <c r="H88" s="8"/>
+      <c r="I88" s="35"/>
     </row>
     <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A89" s="17"/>
-      <c r="B89" s="17"/>
-      <c r="C89" s="17"/>
-      <c r="D89" s="21"/>
-      <c r="E89" s="22"/>
+      <c r="A89" s="8"/>
+      <c r="B89" s="8"/>
+      <c r="C89" s="8"/>
+      <c r="D89" s="20"/>
+      <c r="E89" s="21"/>
       <c r="F89" s="5"/>
-      <c r="G89" s="17"/>
-      <c r="H89" s="17"/>
-      <c r="I89" s="26"/>
+      <c r="G89" s="8"/>
+      <c r="H89" s="8"/>
+      <c r="I89" s="35"/>
     </row>
     <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A90" s="18"/>
-      <c r="B90" s="18"/>
-      <c r="C90" s="18"/>
-      <c r="D90" s="23"/>
-      <c r="E90" s="24"/>
+      <c r="A90" s="9"/>
+      <c r="B90" s="9"/>
+      <c r="C90" s="9"/>
+      <c r="D90" s="22"/>
+      <c r="E90" s="23"/>
       <c r="F90" s="5"/>
-      <c r="G90" s="18"/>
-      <c r="H90" s="18"/>
-      <c r="I90" s="27"/>
+      <c r="G90" s="9"/>
+      <c r="H90" s="9"/>
+      <c r="I90" s="36"/>
     </row>
     <row r="91" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A91" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B91" s="30" t="s">
+      <c r="B91" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C91" s="31"/>
+      <c r="C91" s="17"/>
       <c r="D91" s="4" t="s">
         <v>2</v>
       </c>
@@ -2616,151 +2619,151 @@
       </c>
     </row>
     <row r="92" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="16">
+      <c r="A92" s="27">
         <v>9</v>
       </c>
-      <c r="B92" s="19" t="s">
-        <v>74</v>
-      </c>
-      <c r="C92" s="20"/>
-      <c r="D92" s="10" t="s">
+      <c r="B92" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="E92" s="10" t="s">
+      <c r="C92" s="19"/>
+      <c r="D92" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E92" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F92" s="13" t="s">
+      <c r="F92" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="G92" s="10" t="s">
+      <c r="G92" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H92" s="10" t="s">
+      <c r="H92" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I92" s="10" t="s">
+      <c r="I92" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="93" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="17"/>
-      <c r="B93" s="21"/>
-      <c r="C93" s="22"/>
-      <c r="D93" s="17"/>
-      <c r="E93" s="17"/>
-      <c r="F93" s="14"/>
-      <c r="G93" s="17"/>
-      <c r="H93" s="17"/>
-      <c r="I93" s="26"/>
+      <c r="A93" s="8"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="21"/>
+      <c r="D93" s="8"/>
+      <c r="E93" s="8"/>
+      <c r="F93" s="15"/>
+      <c r="G93" s="8"/>
+      <c r="H93" s="8"/>
+      <c r="I93" s="35"/>
     </row>
     <row r="94" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="17"/>
-      <c r="B94" s="23"/>
-      <c r="C94" s="24"/>
-      <c r="D94" s="17"/>
-      <c r="E94" s="17"/>
+      <c r="A94" s="8"/>
+      <c r="B94" s="22"/>
+      <c r="C94" s="23"/>
+      <c r="D94" s="8"/>
+      <c r="E94" s="8"/>
       <c r="F94" s="5"/>
-      <c r="G94" s="17"/>
-      <c r="H94" s="17"/>
-      <c r="I94" s="26"/>
+      <c r="G94" s="8"/>
+      <c r="H94" s="8"/>
+      <c r="I94" s="35"/>
     </row>
     <row r="95" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="17"/>
-      <c r="B95" s="32" t="s">
+      <c r="A95" s="8"/>
+      <c r="B95" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C95" s="33" t="s">
+      <c r="C95" s="29" t="s">
         <v>47</v>
       </c>
-      <c r="D95" s="17"/>
-      <c r="E95" s="17"/>
+      <c r="D95" s="8"/>
+      <c r="E95" s="8"/>
       <c r="F95" s="5"/>
-      <c r="G95" s="17"/>
-      <c r="H95" s="17"/>
-      <c r="I95" s="26"/>
+      <c r="G95" s="8"/>
+      <c r="H95" s="8"/>
+      <c r="I95" s="35"/>
     </row>
     <row r="96" spans="1:9" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="17"/>
-      <c r="B96" s="18"/>
-      <c r="C96" s="18"/>
-      <c r="D96" s="18"/>
-      <c r="E96" s="18"/>
+      <c r="A96" s="8"/>
+      <c r="B96" s="9"/>
+      <c r="C96" s="9"/>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
       <c r="F96" s="5"/>
-      <c r="G96" s="17"/>
-      <c r="H96" s="17"/>
-      <c r="I96" s="26"/>
+      <c r="G96" s="8"/>
+      <c r="H96" s="8"/>
+      <c r="I96" s="35"/>
     </row>
     <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A97" s="17"/>
-      <c r="B97" s="28" t="s">
+      <c r="A97" s="8"/>
+      <c r="B97" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C97" s="29" t="s">
+      <c r="C97" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="D97" s="34" t="s">
+      <c r="D97" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E97" s="31"/>
+      <c r="E97" s="17"/>
       <c r="F97" s="5"/>
-      <c r="G97" s="17"/>
-      <c r="H97" s="17"/>
-      <c r="I97" s="26"/>
+      <c r="G97" s="8"/>
+      <c r="H97" s="8"/>
+      <c r="I97" s="35"/>
     </row>
     <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A98" s="17"/>
-      <c r="B98" s="17"/>
-      <c r="C98" s="17"/>
-      <c r="D98" s="35" t="s">
+      <c r="A98" s="8"/>
+      <c r="B98" s="8"/>
+      <c r="C98" s="8"/>
+      <c r="D98" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E98" s="20"/>
+      <c r="E98" s="19"/>
       <c r="F98" s="5"/>
-      <c r="G98" s="17"/>
-      <c r="H98" s="17"/>
-      <c r="I98" s="26"/>
+      <c r="G98" s="8"/>
+      <c r="H98" s="8"/>
+      <c r="I98" s="35"/>
     </row>
     <row r="99" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A99" s="17"/>
-      <c r="B99" s="17"/>
-      <c r="C99" s="17"/>
-      <c r="D99" s="21"/>
-      <c r="E99" s="22"/>
+      <c r="A99" s="8"/>
+      <c r="B99" s="8"/>
+      <c r="C99" s="8"/>
+      <c r="D99" s="20"/>
+      <c r="E99" s="21"/>
       <c r="F99" s="5"/>
-      <c r="G99" s="17"/>
-      <c r="H99" s="17"/>
-      <c r="I99" s="26"/>
+      <c r="G99" s="8"/>
+      <c r="H99" s="8"/>
+      <c r="I99" s="35"/>
     </row>
     <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A100" s="17"/>
-      <c r="B100" s="17"/>
-      <c r="C100" s="17"/>
-      <c r="D100" s="21"/>
-      <c r="E100" s="22"/>
+      <c r="A100" s="8"/>
+      <c r="B100" s="8"/>
+      <c r="C100" s="8"/>
+      <c r="D100" s="20"/>
+      <c r="E100" s="21"/>
       <c r="F100" s="5"/>
-      <c r="G100" s="17"/>
-      <c r="H100" s="17"/>
-      <c r="I100" s="26"/>
+      <c r="G100" s="8"/>
+      <c r="H100" s="8"/>
+      <c r="I100" s="35"/>
     </row>
     <row r="101" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A101" s="18"/>
-      <c r="B101" s="18"/>
-      <c r="C101" s="18"/>
-      <c r="D101" s="23"/>
-      <c r="E101" s="24"/>
+      <c r="A101" s="9"/>
+      <c r="B101" s="9"/>
+      <c r="C101" s="9"/>
+      <c r="D101" s="22"/>
+      <c r="E101" s="23"/>
       <c r="F101" s="5"/>
-      <c r="G101" s="18"/>
-      <c r="H101" s="18"/>
-      <c r="I101" s="27"/>
+      <c r="G101" s="9"/>
+      <c r="H101" s="9"/>
+      <c r="I101" s="36"/>
     </row>
     <row r="102" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A102" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B102" s="30" t="s">
+      <c r="B102" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C102" s="31"/>
+      <c r="C102" s="17"/>
       <c r="D102" s="4" t="s">
         <v>2</v>
       </c>
@@ -2781,149 +2784,149 @@
       </c>
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A103" s="16">
+      <c r="A103" s="27">
         <v>10</v>
       </c>
-      <c r="B103" s="19" t="s">
+      <c r="B103" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="C103" s="20"/>
-      <c r="D103" s="10" t="s">
-        <v>75</v>
-      </c>
-      <c r="E103" s="10" t="s">
+      <c r="C103" s="19"/>
+      <c r="D103" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="E103" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="F103" s="13" t="s">
+      <c r="F103" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="G103" s="10" t="s">
+      <c r="G103" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H103" s="10" t="s">
+      <c r="H103" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="I103" s="25"/>
+      <c r="I103" s="10"/>
     </row>
     <row r="104" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="17"/>
-      <c r="B104" s="21"/>
-      <c r="C104" s="22"/>
-      <c r="D104" s="17"/>
-      <c r="E104" s="17"/>
-      <c r="F104" s="14"/>
-      <c r="G104" s="17"/>
-      <c r="H104" s="17"/>
-      <c r="I104" s="17"/>
+      <c r="A104" s="8"/>
+      <c r="B104" s="20"/>
+      <c r="C104" s="21"/>
+      <c r="D104" s="8"/>
+      <c r="E104" s="8"/>
+      <c r="F104" s="15"/>
+      <c r="G104" s="8"/>
+      <c r="H104" s="8"/>
+      <c r="I104" s="8"/>
     </row>
     <row r="105" spans="1:9" ht="59.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="17"/>
-      <c r="B105" s="23"/>
-      <c r="C105" s="24"/>
-      <c r="D105" s="17"/>
-      <c r="E105" s="17"/>
+      <c r="A105" s="8"/>
+      <c r="B105" s="22"/>
+      <c r="C105" s="23"/>
+      <c r="D105" s="8"/>
+      <c r="E105" s="8"/>
       <c r="F105" s="5"/>
-      <c r="G105" s="17"/>
-      <c r="H105" s="17"/>
-      <c r="I105" s="17"/>
+      <c r="G105" s="8"/>
+      <c r="H105" s="8"/>
+      <c r="I105" s="8"/>
     </row>
     <row r="106" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="17"/>
-      <c r="B106" s="32" t="s">
+      <c r="A106" s="8"/>
+      <c r="B106" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C106" s="42" t="s">
+      <c r="C106" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="D106" s="17"/>
-      <c r="E106" s="17"/>
+      <c r="D106" s="8"/>
+      <c r="E106" s="8"/>
       <c r="F106" s="5"/>
-      <c r="G106" s="17"/>
-      <c r="H106" s="17"/>
-      <c r="I106" s="17"/>
+      <c r="G106" s="8"/>
+      <c r="H106" s="8"/>
+      <c r="I106" s="8"/>
     </row>
     <row r="107" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="17"/>
-      <c r="B107" s="18"/>
-      <c r="C107" s="43"/>
-      <c r="D107" s="18"/>
-      <c r="E107" s="18"/>
+      <c r="A107" s="8"/>
+      <c r="B107" s="9"/>
+      <c r="C107" s="13"/>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9"/>
       <c r="F107" s="5"/>
-      <c r="G107" s="17"/>
-      <c r="H107" s="17"/>
-      <c r="I107" s="17"/>
+      <c r="G107" s="8"/>
+      <c r="H107" s="8"/>
+      <c r="I107" s="8"/>
     </row>
     <row r="108" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A108" s="17"/>
-      <c r="B108" s="28" t="s">
+      <c r="A108" s="8"/>
+      <c r="B108" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C108" s="29" t="s">
+      <c r="C108" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="D108" s="34" t="s">
+      <c r="D108" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E108" s="31"/>
+      <c r="E108" s="17"/>
       <c r="F108" s="5"/>
-      <c r="G108" s="17"/>
-      <c r="H108" s="17"/>
-      <c r="I108" s="17"/>
+      <c r="G108" s="8"/>
+      <c r="H108" s="8"/>
+      <c r="I108" s="8"/>
     </row>
     <row r="109" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="17"/>
-      <c r="B109" s="17"/>
-      <c r="C109" s="17"/>
-      <c r="D109" s="35" t="s">
+      <c r="A109" s="8"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="8"/>
+      <c r="D109" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E109" s="20"/>
+      <c r="E109" s="19"/>
       <c r="F109" s="5"/>
-      <c r="G109" s="17"/>
-      <c r="H109" s="17"/>
-      <c r="I109" s="17"/>
+      <c r="G109" s="8"/>
+      <c r="H109" s="8"/>
+      <c r="I109" s="8"/>
     </row>
     <row r="110" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="17"/>
-      <c r="B110" s="17"/>
-      <c r="C110" s="17"/>
-      <c r="D110" s="21"/>
-      <c r="E110" s="22"/>
+      <c r="A110" s="8"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="8"/>
+      <c r="D110" s="20"/>
+      <c r="E110" s="21"/>
       <c r="F110" s="5"/>
-      <c r="G110" s="17"/>
-      <c r="H110" s="17"/>
-      <c r="I110" s="17"/>
+      <c r="G110" s="8"/>
+      <c r="H110" s="8"/>
+      <c r="I110" s="8"/>
     </row>
     <row r="111" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="17"/>
-      <c r="B111" s="17"/>
-      <c r="C111" s="17"/>
-      <c r="D111" s="21"/>
-      <c r="E111" s="22"/>
+      <c r="A111" s="8"/>
+      <c r="B111" s="8"/>
+      <c r="C111" s="8"/>
+      <c r="D111" s="20"/>
+      <c r="E111" s="21"/>
       <c r="F111" s="5"/>
-      <c r="G111" s="17"/>
-      <c r="H111" s="17"/>
-      <c r="I111" s="17"/>
+      <c r="G111" s="8"/>
+      <c r="H111" s="8"/>
+      <c r="I111" s="8"/>
     </row>
     <row r="112" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="18"/>
-      <c r="B112" s="18"/>
-      <c r="C112" s="18"/>
-      <c r="D112" s="23"/>
-      <c r="E112" s="24"/>
+      <c r="A112" s="9"/>
+      <c r="B112" s="9"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="22"/>
+      <c r="E112" s="23"/>
       <c r="F112" s="5"/>
-      <c r="G112" s="18"/>
-      <c r="H112" s="18"/>
-      <c r="I112" s="18"/>
+      <c r="G112" s="9"/>
+      <c r="H112" s="9"/>
+      <c r="I112" s="9"/>
     </row>
     <row r="113" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B113" s="30" t="s">
+      <c r="B113" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C113" s="31"/>
+      <c r="C113" s="17"/>
       <c r="D113" s="4" t="s">
         <v>2</v>
       </c>
@@ -2944,130 +2947,130 @@
       </c>
     </row>
     <row r="114" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A114" s="16">
+      <c r="A114" s="27">
         <v>11</v>
       </c>
-      <c r="B114" s="19"/>
-      <c r="C114" s="20"/>
-      <c r="D114" s="10"/>
-      <c r="E114" s="10"/>
-      <c r="G114" s="10"/>
-      <c r="H114" s="10"/>
-      <c r="I114" s="25"/>
+      <c r="B114" s="28"/>
+      <c r="C114" s="19"/>
+      <c r="D114" s="7"/>
+      <c r="E114" s="7"/>
+      <c r="G114" s="7"/>
+      <c r="H114" s="7"/>
+      <c r="I114" s="10"/>
     </row>
     <row r="115" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A115" s="17"/>
-      <c r="B115" s="21"/>
-      <c r="C115" s="22"/>
-      <c r="D115" s="17"/>
-      <c r="E115" s="17"/>
+      <c r="A115" s="8"/>
+      <c r="B115" s="20"/>
+      <c r="C115" s="21"/>
+      <c r="D115" s="8"/>
+      <c r="E115" s="8"/>
       <c r="F115" s="5"/>
-      <c r="G115" s="17"/>
-      <c r="H115" s="17"/>
-      <c r="I115" s="17"/>
+      <c r="G115" s="8"/>
+      <c r="H115" s="8"/>
+      <c r="I115" s="8"/>
     </row>
     <row r="116" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A116" s="17"/>
-      <c r="B116" s="23"/>
-      <c r="C116" s="24"/>
-      <c r="D116" s="17"/>
-      <c r="E116" s="17"/>
+      <c r="A116" s="8"/>
+      <c r="B116" s="22"/>
+      <c r="C116" s="23"/>
+      <c r="D116" s="8"/>
+      <c r="E116" s="8"/>
       <c r="F116" s="5"/>
-      <c r="G116" s="17"/>
-      <c r="H116" s="17"/>
-      <c r="I116" s="17"/>
+      <c r="G116" s="8"/>
+      <c r="H116" s="8"/>
+      <c r="I116" s="8"/>
     </row>
     <row r="117" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A117" s="17"/>
-      <c r="B117" s="32" t="s">
+      <c r="A117" s="8"/>
+      <c r="B117" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C117" s="33"/>
-      <c r="D117" s="17"/>
-      <c r="E117" s="17"/>
+      <c r="C117" s="29"/>
+      <c r="D117" s="8"/>
+      <c r="E117" s="8"/>
       <c r="F117" s="5"/>
-      <c r="G117" s="17"/>
-      <c r="H117" s="17"/>
-      <c r="I117" s="17"/>
+      <c r="G117" s="8"/>
+      <c r="H117" s="8"/>
+      <c r="I117" s="8"/>
     </row>
     <row r="118" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A118" s="17"/>
-      <c r="B118" s="18"/>
-      <c r="C118" s="18"/>
-      <c r="D118" s="18"/>
-      <c r="E118" s="18"/>
+      <c r="A118" s="8"/>
+      <c r="B118" s="9"/>
+      <c r="C118" s="9"/>
+      <c r="D118" s="9"/>
+      <c r="E118" s="9"/>
       <c r="F118" s="5"/>
-      <c r="G118" s="17"/>
-      <c r="H118" s="17"/>
-      <c r="I118" s="17"/>
+      <c r="G118" s="8"/>
+      <c r="H118" s="8"/>
+      <c r="I118" s="8"/>
     </row>
     <row r="119" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A119" s="17"/>
-      <c r="B119" s="28" t="s">
+      <c r="A119" s="8"/>
+      <c r="B119" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C119" s="29"/>
-      <c r="D119" s="34" t="s">
+      <c r="C119" s="25"/>
+      <c r="D119" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E119" s="31"/>
+      <c r="E119" s="17"/>
       <c r="F119" s="5"/>
-      <c r="G119" s="17"/>
-      <c r="H119" s="17"/>
-      <c r="I119" s="17"/>
+      <c r="G119" s="8"/>
+      <c r="H119" s="8"/>
+      <c r="I119" s="8"/>
     </row>
     <row r="120" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A120" s="17"/>
-      <c r="B120" s="17"/>
-      <c r="C120" s="17"/>
-      <c r="D120" s="35"/>
-      <c r="E120" s="20"/>
+      <c r="A120" s="8"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="8"/>
+      <c r="D120" s="18"/>
+      <c r="E120" s="19"/>
       <c r="F120" s="5"/>
-      <c r="G120" s="17"/>
-      <c r="H120" s="17"/>
-      <c r="I120" s="17"/>
+      <c r="G120" s="8"/>
+      <c r="H120" s="8"/>
+      <c r="I120" s="8"/>
     </row>
     <row r="121" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A121" s="17"/>
-      <c r="B121" s="17"/>
-      <c r="C121" s="17"/>
-      <c r="D121" s="21"/>
-      <c r="E121" s="22"/>
+      <c r="A121" s="8"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="8"/>
+      <c r="D121" s="20"/>
+      <c r="E121" s="21"/>
       <c r="F121" s="5"/>
-      <c r="G121" s="17"/>
-      <c r="H121" s="17"/>
-      <c r="I121" s="17"/>
+      <c r="G121" s="8"/>
+      <c r="H121" s="8"/>
+      <c r="I121" s="8"/>
     </row>
     <row r="122" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A122" s="17"/>
-      <c r="B122" s="17"/>
-      <c r="C122" s="17"/>
-      <c r="D122" s="21"/>
-      <c r="E122" s="22"/>
+      <c r="A122" s="8"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="8"/>
+      <c r="D122" s="20"/>
+      <c r="E122" s="21"/>
       <c r="F122" s="5"/>
-      <c r="G122" s="17"/>
-      <c r="H122" s="17"/>
-      <c r="I122" s="17"/>
+      <c r="G122" s="8"/>
+      <c r="H122" s="8"/>
+      <c r="I122" s="8"/>
     </row>
     <row r="123" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A123" s="18"/>
-      <c r="B123" s="18"/>
-      <c r="C123" s="18"/>
-      <c r="D123" s="23"/>
-      <c r="E123" s="24"/>
+      <c r="A123" s="9"/>
+      <c r="B123" s="9"/>
+      <c r="C123" s="9"/>
+      <c r="D123" s="22"/>
+      <c r="E123" s="23"/>
       <c r="F123" s="5"/>
-      <c r="G123" s="18"/>
-      <c r="H123" s="18"/>
-      <c r="I123" s="18"/>
+      <c r="G123" s="9"/>
+      <c r="H123" s="9"/>
+      <c r="I123" s="9"/>
     </row>
     <row r="124" spans="1:9" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A124" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B124" s="30" t="s">
+      <c r="B124" s="26" t="s">
         <v>1</v>
       </c>
-      <c r="C124" s="31"/>
+      <c r="C124" s="17"/>
       <c r="D124" s="4" t="s">
         <v>2</v>
       </c>
@@ -3088,134 +3091,271 @@
       </c>
     </row>
     <row r="125" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A125" s="16">
+      <c r="A125" s="27">
         <v>12</v>
       </c>
-      <c r="B125" s="19"/>
-      <c r="C125" s="20"/>
-      <c r="D125" s="10"/>
-      <c r="E125" s="10"/>
-      <c r="G125" s="10"/>
-      <c r="H125" s="10"/>
-      <c r="I125" s="25"/>
+      <c r="B125" s="28"/>
+      <c r="C125" s="19"/>
+      <c r="D125" s="7"/>
+      <c r="E125" s="7"/>
+      <c r="G125" s="7"/>
+      <c r="H125" s="7"/>
+      <c r="I125" s="10"/>
     </row>
     <row r="126" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A126" s="17"/>
-      <c r="B126" s="21"/>
-      <c r="C126" s="22"/>
-      <c r="D126" s="17"/>
-      <c r="E126" s="17"/>
+      <c r="A126" s="8"/>
+      <c r="B126" s="20"/>
+      <c r="C126" s="21"/>
+      <c r="D126" s="8"/>
+      <c r="E126" s="8"/>
       <c r="F126" s="5"/>
-      <c r="G126" s="17"/>
-      <c r="H126" s="17"/>
-      <c r="I126" s="17"/>
+      <c r="G126" s="8"/>
+      <c r="H126" s="8"/>
+      <c r="I126" s="8"/>
     </row>
     <row r="127" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A127" s="17"/>
-      <c r="B127" s="23"/>
-      <c r="C127" s="24"/>
-      <c r="D127" s="17"/>
-      <c r="E127" s="17"/>
+      <c r="A127" s="8"/>
+      <c r="B127" s="22"/>
+      <c r="C127" s="23"/>
+      <c r="D127" s="8"/>
+      <c r="E127" s="8"/>
       <c r="F127" s="5"/>
-      <c r="G127" s="17"/>
-      <c r="H127" s="17"/>
-      <c r="I127" s="17"/>
+      <c r="G127" s="8"/>
+      <c r="H127" s="8"/>
+      <c r="I127" s="8"/>
     </row>
     <row r="128" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A128" s="17"/>
-      <c r="B128" s="32" t="s">
+      <c r="A128" s="8"/>
+      <c r="B128" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="C128" s="33"/>
-      <c r="D128" s="17"/>
-      <c r="E128" s="17"/>
+      <c r="C128" s="29"/>
+      <c r="D128" s="8"/>
+      <c r="E128" s="8"/>
       <c r="F128" s="5"/>
-      <c r="G128" s="17"/>
-      <c r="H128" s="17"/>
-      <c r="I128" s="17"/>
+      <c r="G128" s="8"/>
+      <c r="H128" s="8"/>
+      <c r="I128" s="8"/>
     </row>
     <row r="129" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A129" s="17"/>
-      <c r="B129" s="18"/>
-      <c r="C129" s="18"/>
-      <c r="D129" s="18"/>
-      <c r="E129" s="18"/>
+      <c r="A129" s="8"/>
+      <c r="B129" s="9"/>
+      <c r="C129" s="9"/>
+      <c r="D129" s="9"/>
+      <c r="E129" s="9"/>
       <c r="F129" s="5"/>
-      <c r="G129" s="17"/>
-      <c r="H129" s="17"/>
-      <c r="I129" s="17"/>
+      <c r="G129" s="8"/>
+      <c r="H129" s="8"/>
+      <c r="I129" s="8"/>
     </row>
     <row r="130" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A130" s="17"/>
-      <c r="B130" s="28" t="s">
+      <c r="A130" s="8"/>
+      <c r="B130" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="C130" s="29"/>
-      <c r="D130" s="34" t="s">
+      <c r="C130" s="25"/>
+      <c r="D130" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="E130" s="31"/>
+      <c r="E130" s="17"/>
       <c r="F130" s="5"/>
-      <c r="G130" s="17"/>
-      <c r="H130" s="17"/>
-      <c r="I130" s="17"/>
+      <c r="G130" s="8"/>
+      <c r="H130" s="8"/>
+      <c r="I130" s="8"/>
     </row>
     <row r="131" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A131" s="17"/>
-      <c r="B131" s="17"/>
-      <c r="C131" s="17"/>
-      <c r="D131" s="35"/>
-      <c r="E131" s="20"/>
+      <c r="A131" s="8"/>
+      <c r="B131" s="8"/>
+      <c r="C131" s="8"/>
+      <c r="D131" s="18"/>
+      <c r="E131" s="19"/>
       <c r="F131" s="5"/>
-      <c r="G131" s="17"/>
-      <c r="H131" s="17"/>
-      <c r="I131" s="17"/>
+      <c r="G131" s="8"/>
+      <c r="H131" s="8"/>
+      <c r="I131" s="8"/>
     </row>
     <row r="132" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A132" s="17"/>
-      <c r="B132" s="17"/>
-      <c r="C132" s="17"/>
-      <c r="D132" s="21"/>
-      <c r="E132" s="22"/>
+      <c r="A132" s="8"/>
+      <c r="B132" s="8"/>
+      <c r="C132" s="8"/>
+      <c r="D132" s="20"/>
+      <c r="E132" s="21"/>
       <c r="F132" s="5"/>
-      <c r="G132" s="17"/>
-      <c r="H132" s="17"/>
-      <c r="I132" s="17"/>
+      <c r="G132" s="8"/>
+      <c r="H132" s="8"/>
+      <c r="I132" s="8"/>
     </row>
     <row r="133" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A133" s="17"/>
-      <c r="B133" s="17"/>
-      <c r="C133" s="17"/>
-      <c r="D133" s="21"/>
-      <c r="E133" s="22"/>
+      <c r="A133" s="8"/>
+      <c r="B133" s="8"/>
+      <c r="C133" s="8"/>
+      <c r="D133" s="20"/>
+      <c r="E133" s="21"/>
       <c r="F133" s="5"/>
-      <c r="G133" s="17"/>
-      <c r="H133" s="17"/>
-      <c r="I133" s="17"/>
+      <c r="G133" s="8"/>
+      <c r="H133" s="8"/>
+      <c r="I133" s="8"/>
     </row>
     <row r="134" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A134" s="18"/>
-      <c r="B134" s="18"/>
-      <c r="C134" s="18"/>
-      <c r="D134" s="23"/>
-      <c r="E134" s="24"/>
+      <c r="A134" s="9"/>
+      <c r="B134" s="9"/>
+      <c r="C134" s="9"/>
+      <c r="D134" s="22"/>
+      <c r="E134" s="23"/>
       <c r="F134" s="5"/>
-      <c r="G134" s="18"/>
-      <c r="H134" s="18"/>
-      <c r="I134" s="18"/>
+      <c r="G134" s="9"/>
+      <c r="H134" s="9"/>
+      <c r="I134" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="181">
-    <mergeCell ref="G103:G112"/>
-    <mergeCell ref="H103:H112"/>
-    <mergeCell ref="I103:I112"/>
-    <mergeCell ref="B106:B107"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="F103:F104"/>
-    <mergeCell ref="D108:E108"/>
-    <mergeCell ref="D109:E112"/>
-    <mergeCell ref="B108:B112"/>
-    <mergeCell ref="C108:C112"/>
+    <mergeCell ref="A114:A123"/>
+    <mergeCell ref="B114:C116"/>
+    <mergeCell ref="D114:D118"/>
+    <mergeCell ref="E114:E118"/>
+    <mergeCell ref="A92:A101"/>
+    <mergeCell ref="B84:B85"/>
+    <mergeCell ref="C84:C85"/>
+    <mergeCell ref="A81:A90"/>
+    <mergeCell ref="B81:C83"/>
+    <mergeCell ref="D81:D85"/>
+    <mergeCell ref="E81:E85"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="D97:E97"/>
+    <mergeCell ref="D98:E101"/>
+    <mergeCell ref="D86:E86"/>
+    <mergeCell ref="D87:E90"/>
+    <mergeCell ref="D92:D96"/>
+    <mergeCell ref="E92:E96"/>
+    <mergeCell ref="G81:G90"/>
+    <mergeCell ref="H81:H90"/>
+    <mergeCell ref="B86:B90"/>
+    <mergeCell ref="C86:C90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="F92:F93"/>
+    <mergeCell ref="B97:B101"/>
+    <mergeCell ref="C97:C101"/>
+    <mergeCell ref="F59:F60"/>
+    <mergeCell ref="G70:G79"/>
+    <mergeCell ref="H70:H79"/>
+    <mergeCell ref="I70:I79"/>
+    <mergeCell ref="F70:F71"/>
+    <mergeCell ref="G114:G123"/>
+    <mergeCell ref="H114:H123"/>
+    <mergeCell ref="I114:I123"/>
+    <mergeCell ref="G92:G101"/>
+    <mergeCell ref="H92:H101"/>
+    <mergeCell ref="I92:I101"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="A26:A35"/>
+    <mergeCell ref="B26:C28"/>
+    <mergeCell ref="D26:D30"/>
+    <mergeCell ref="E26:E30"/>
+    <mergeCell ref="I81:I90"/>
+    <mergeCell ref="F81:F84"/>
+    <mergeCell ref="B75:B79"/>
+    <mergeCell ref="C75:C79"/>
+    <mergeCell ref="B80:C80"/>
+    <mergeCell ref="B64:B68"/>
+    <mergeCell ref="C64:C68"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="A70:A79"/>
+    <mergeCell ref="B70:C72"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="A59:A68"/>
+    <mergeCell ref="B59:C61"/>
+    <mergeCell ref="D59:D63"/>
+    <mergeCell ref="E59:E63"/>
+    <mergeCell ref="G59:G68"/>
+    <mergeCell ref="H59:H68"/>
+    <mergeCell ref="I59:I68"/>
+    <mergeCell ref="A37:A46"/>
+    <mergeCell ref="B37:C39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="A48:A57"/>
+    <mergeCell ref="D75:E75"/>
+    <mergeCell ref="D76:E79"/>
+    <mergeCell ref="D64:E64"/>
+    <mergeCell ref="D65:E68"/>
+    <mergeCell ref="D70:D74"/>
+    <mergeCell ref="E70:E74"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D54:E57"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="D43:E46"/>
+    <mergeCell ref="D48:D52"/>
+    <mergeCell ref="E48:E52"/>
+    <mergeCell ref="B62:B63"/>
+    <mergeCell ref="C62:C63"/>
+    <mergeCell ref="B53:B57"/>
+    <mergeCell ref="C53:C57"/>
+    <mergeCell ref="B58:C58"/>
+    <mergeCell ref="G48:G57"/>
+    <mergeCell ref="H48:H57"/>
+    <mergeCell ref="I48:I57"/>
+    <mergeCell ref="D37:D41"/>
+    <mergeCell ref="E37:E41"/>
+    <mergeCell ref="G37:G46"/>
+    <mergeCell ref="H37:H46"/>
+    <mergeCell ref="I37:I46"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B42:B46"/>
+    <mergeCell ref="B48:C50"/>
+    <mergeCell ref="F37:F40"/>
+    <mergeCell ref="F48:F50"/>
+    <mergeCell ref="H4:H13"/>
+    <mergeCell ref="I4:I13"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="G26:G35"/>
+    <mergeCell ref="H26:H35"/>
+    <mergeCell ref="I26:I35"/>
+    <mergeCell ref="D31:E31"/>
+    <mergeCell ref="D32:E35"/>
+    <mergeCell ref="I15:I24"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="C9:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="F4:F7"/>
+    <mergeCell ref="F8:F10"/>
+    <mergeCell ref="F15:F16"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="A1:I2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="A4:A13"/>
+    <mergeCell ref="B4:C6"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="E4:E8"/>
+    <mergeCell ref="G4:G13"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="D20:E20"/>
+    <mergeCell ref="D21:E24"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="D10:E13"/>
+    <mergeCell ref="D15:D19"/>
+    <mergeCell ref="E15:E19"/>
+    <mergeCell ref="G15:G24"/>
+    <mergeCell ref="H15:H24"/>
+    <mergeCell ref="A15:A24"/>
+    <mergeCell ref="B15:C17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
     <mergeCell ref="B113:C113"/>
     <mergeCell ref="A103:A112"/>
     <mergeCell ref="B103:C105"/>
@@ -3240,153 +3380,16 @@
     <mergeCell ref="D130:E130"/>
     <mergeCell ref="D131:E134"/>
     <mergeCell ref="B117:B118"/>
-    <mergeCell ref="C117:C118"/>
-    <mergeCell ref="A1:I2"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="A4:A13"/>
-    <mergeCell ref="B4:C6"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="E4:E8"/>
-    <mergeCell ref="G4:G13"/>
-    <mergeCell ref="B20:B24"/>
-    <mergeCell ref="C20:C24"/>
-    <mergeCell ref="D20:E20"/>
-    <mergeCell ref="D21:E24"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D10:E13"/>
-    <mergeCell ref="D15:D19"/>
-    <mergeCell ref="E15:E19"/>
-    <mergeCell ref="G15:G24"/>
-    <mergeCell ref="H15:H24"/>
-    <mergeCell ref="A15:A24"/>
-    <mergeCell ref="B15:C17"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="H4:H13"/>
-    <mergeCell ref="I4:I13"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B25:C25"/>
-    <mergeCell ref="G26:G35"/>
-    <mergeCell ref="H26:H35"/>
-    <mergeCell ref="I26:I35"/>
-    <mergeCell ref="D31:E31"/>
-    <mergeCell ref="D32:E35"/>
-    <mergeCell ref="I15:I24"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="G48:G57"/>
-    <mergeCell ref="H48:H57"/>
-    <mergeCell ref="I48:I57"/>
-    <mergeCell ref="D37:D41"/>
-    <mergeCell ref="E37:E41"/>
-    <mergeCell ref="G37:G46"/>
-    <mergeCell ref="H37:H46"/>
-    <mergeCell ref="I37:I46"/>
-    <mergeCell ref="C42:C46"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="B48:C50"/>
-    <mergeCell ref="C31:C35"/>
-    <mergeCell ref="A37:A46"/>
-    <mergeCell ref="B37:C39"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A48:A57"/>
-    <mergeCell ref="D75:E75"/>
-    <mergeCell ref="D76:E79"/>
-    <mergeCell ref="D64:E64"/>
-    <mergeCell ref="D65:E68"/>
-    <mergeCell ref="D70:D74"/>
-    <mergeCell ref="E70:E74"/>
-    <mergeCell ref="D53:E53"/>
-    <mergeCell ref="D54:E57"/>
-    <mergeCell ref="D42:E42"/>
-    <mergeCell ref="D43:E46"/>
-    <mergeCell ref="D48:D52"/>
-    <mergeCell ref="E48:E52"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="A26:A35"/>
-    <mergeCell ref="B26:C28"/>
-    <mergeCell ref="D26:D30"/>
-    <mergeCell ref="E26:E30"/>
-    <mergeCell ref="I81:I90"/>
-    <mergeCell ref="F81:F84"/>
-    <mergeCell ref="B75:B79"/>
-    <mergeCell ref="C75:C79"/>
-    <mergeCell ref="B80:C80"/>
-    <mergeCell ref="B64:B68"/>
-    <mergeCell ref="C64:C68"/>
-    <mergeCell ref="B69:C69"/>
-    <mergeCell ref="A70:A79"/>
-    <mergeCell ref="B70:C72"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="A59:A68"/>
-    <mergeCell ref="B59:C61"/>
-    <mergeCell ref="D59:D63"/>
-    <mergeCell ref="E59:E63"/>
-    <mergeCell ref="G59:G68"/>
-    <mergeCell ref="H59:H68"/>
-    <mergeCell ref="I59:I68"/>
-    <mergeCell ref="F59:F60"/>
-    <mergeCell ref="G70:G79"/>
-    <mergeCell ref="H70:H79"/>
-    <mergeCell ref="I70:I79"/>
-    <mergeCell ref="F70:F71"/>
-    <mergeCell ref="G114:G123"/>
-    <mergeCell ref="H114:H123"/>
-    <mergeCell ref="I114:I123"/>
-    <mergeCell ref="G92:G101"/>
-    <mergeCell ref="H92:H101"/>
-    <mergeCell ref="I92:I101"/>
-    <mergeCell ref="B86:B90"/>
-    <mergeCell ref="C86:C90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="C95:C96"/>
-    <mergeCell ref="F92:F93"/>
-    <mergeCell ref="B97:B101"/>
-    <mergeCell ref="C97:C101"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="D97:E97"/>
-    <mergeCell ref="D98:E101"/>
-    <mergeCell ref="D86:E86"/>
-    <mergeCell ref="D87:E90"/>
-    <mergeCell ref="D92:D96"/>
-    <mergeCell ref="E92:E96"/>
-    <mergeCell ref="G81:G90"/>
-    <mergeCell ref="H81:H90"/>
-    <mergeCell ref="F4:F7"/>
-    <mergeCell ref="F8:F10"/>
-    <mergeCell ref="F15:F16"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="F37:F40"/>
-    <mergeCell ref="F48:F50"/>
-    <mergeCell ref="A114:A123"/>
-    <mergeCell ref="B114:C116"/>
-    <mergeCell ref="D114:D118"/>
-    <mergeCell ref="E114:E118"/>
-    <mergeCell ref="A92:A101"/>
-    <mergeCell ref="B84:B85"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="A81:A90"/>
-    <mergeCell ref="B81:C83"/>
-    <mergeCell ref="D81:D85"/>
-    <mergeCell ref="E81:E85"/>
-    <mergeCell ref="B62:B63"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="B53:B57"/>
-    <mergeCell ref="C53:C57"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B31:B35"/>
+    <mergeCell ref="G103:G112"/>
+    <mergeCell ref="H103:H112"/>
+    <mergeCell ref="I103:I112"/>
+    <mergeCell ref="B106:B107"/>
+    <mergeCell ref="C106:C107"/>
+    <mergeCell ref="F103:F104"/>
+    <mergeCell ref="D108:E108"/>
+    <mergeCell ref="D109:E112"/>
+    <mergeCell ref="B108:B112"/>
+    <mergeCell ref="C108:C112"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>